<commit_message>
Actualización de datos 2022
</commit_message>
<xml_diff>
--- a/Prueba/UrgenciaPorCausayEdad.xlsx
+++ b/Prueba/UrgenciaPorCausayEdad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8688ca3d1d320028/Escritorio/Universidad/Semestre 10/rstudio/repositorio-de-prueba/Prueba/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8688ca3d1d320028/Escritorio/Universidad/Semestre 10/rstudio/demanda_urgencia/Prueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{8E0FDDD9-090C-43F3-AE8A-693F2208E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A09E647F-8370-48CB-B8CB-08C9FCD6C5BA}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="8_{8E0FDDD9-090C-43F3-AE8A-693F2208E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{700231F1-8E29-45C2-8A63-49B9DE8579A1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{DB2892A7-5079-4099-98C4-30A44261E59B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{DB2892A7-5079-4099-98C4-30A44261E59B}"/>
   </bookViews>
   <sheets>
     <sheet name="Causa" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -224,11 +224,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -256,10 +269,14 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,7 +594,7 @@
   <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E4" sqref="E4:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,11 +633,11 @@
         <v>44322</v>
       </c>
       <c r="E3" s="1">
-        <v>53363</v>
+        <v>56955</v>
       </c>
       <c r="F3" s="2">
         <f>SUM(B3:E3)</f>
-        <v>215386</v>
+        <v>218978</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -637,11 +654,11 @@
         <v>3827</v>
       </c>
       <c r="E4" s="1">
-        <v>11428</v>
+        <v>12008</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F8" si="0">SUM(B4:E4)</f>
-        <v>32473</v>
+        <v>33053</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -658,11 +675,11 @@
         <v>4348</v>
       </c>
       <c r="E5" s="1">
-        <v>1546</v>
+        <v>1556</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>9594</v>
+        <v>9604</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -679,11 +696,11 @@
         <v>4585</v>
       </c>
       <c r="E6" s="1">
-        <v>4227</v>
+        <v>4551</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>17216</v>
+        <v>17540</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -700,11 +717,11 @@
         <v>8204</v>
       </c>
       <c r="E7" s="1">
-        <v>9342</v>
+        <v>9960</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>42129</v>
+        <v>42747</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -721,11 +738,11 @@
         <v>23358</v>
       </c>
       <c r="E8" s="1">
-        <v>26820</v>
+        <v>28880</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>113918</v>
+        <v>115978</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -742,7 +759,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="A1:C21"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,10 +937,10 @@
       <c r="A16" s="10">
         <v>2021</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="16">
         <v>23358</v>
       </c>
     </row>
@@ -935,7 +952,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="12">
-        <v>11428</v>
+        <v>12008</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -946,7 +963,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="12">
-        <v>1546</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -957,7 +974,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="12">
-        <v>4227</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -968,7 +985,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="12">
-        <v>9342</v>
+        <v>9960</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -979,7 +996,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="12">
-        <v>26820</v>
+        <v>28880</v>
       </c>
     </row>
   </sheetData>
@@ -991,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C1C692-9E52-49E0-AEE6-01F190CE44E9}">
   <dimension ref="A2:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,12 +1047,12 @@
       <c r="D3" s="2">
         <v>44322</v>
       </c>
-      <c r="E3" s="5">
-        <v>53363</v>
+      <c r="E3" s="2">
+        <v>56955</v>
       </c>
       <c r="F3" s="5">
         <f>SUM(B3:E3)</f>
-        <v>215386</v>
+        <v>218978</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1051,12 +1068,12 @@
       <c r="D4" s="2">
         <v>2030</v>
       </c>
-      <c r="E4" s="5">
-        <v>3429</v>
+      <c r="E4" s="2">
+        <v>3688</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" ref="F4:F8" si="0">SUM(B4:E4)</f>
-        <v>11704</v>
+        <v>11963</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1072,12 +1089,12 @@
       <c r="D5" s="2">
         <v>4810</v>
       </c>
-      <c r="E5" s="5">
-        <v>9244</v>
+      <c r="E5" s="2">
+        <v>9880</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>26734</v>
+        <v>27370</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1093,12 +1110,12 @@
       <c r="D6" s="2">
         <v>4920</v>
       </c>
-      <c r="E6" s="5">
-        <v>9911</v>
+      <c r="E6" s="2">
+        <v>10401</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>30857</v>
+        <v>31347</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1114,12 +1131,12 @@
       <c r="D7" s="2">
         <v>23154</v>
       </c>
-      <c r="E7" s="5">
-        <v>21519</v>
+      <c r="E7" s="2">
+        <v>22999</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>104882</v>
+        <v>106362</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1135,12 +1152,12 @@
       <c r="D8" s="2">
         <v>9408</v>
       </c>
-      <c r="E8" s="5">
-        <v>9260</v>
+      <c r="E8" s="2">
+        <v>9987</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>41061</v>
+        <v>41788</v>
       </c>
     </row>
   </sheetData>
@@ -1152,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AA8737-B7B5-4971-A8BC-A2F804E5BFC1}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,8 +1361,8 @@
       <c r="B17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="14">
-        <v>3429</v>
+      <c r="C17" s="11">
+        <v>3688</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1355,8 +1372,8 @@
       <c r="B18" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="14">
-        <v>9244</v>
+      <c r="C18" s="11">
+        <v>9880</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1366,8 +1383,8 @@
       <c r="B19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="14">
-        <v>9911</v>
+      <c r="C19" s="11">
+        <v>10401</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1377,8 +1394,8 @@
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="14">
-        <v>21519</v>
+      <c r="C20" s="11">
+        <v>22999</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1388,8 +1405,8 @@
       <c r="B21" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="14">
-        <v>9260</v>
+      <c r="C21" s="11">
+        <v>9987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>